<commit_message>
Overwritten functionality of export of Purchase Order. Now 2 different dataProviders are responsible for viewing grid on HTML and creating the Excel file.
</commit_message>
<xml_diff>
--- a/uploads/data/import_products.xlsx
+++ b/uploads/data/import_products.xlsx
@@ -19,11 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>SKU</t>
   </si>
   <si>
+    <t>1007e2</t>
+  </si>
+  <si>
     <t>1091e</t>
   </si>
   <si>
@@ -120,10 +123,10 @@
     <t>cognac</t>
   </si>
   <si>
-    <t>4738e9</t>
-  </si>
-  <si>
-    <t>4382B</t>
+    <t>31903</t>
+  </si>
+  <si>
+    <t>Washka Pashka</t>
   </si>
 </sst>
 </file>
@@ -231,15 +234,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -580,7 +583,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -600,90 +603,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
-      <c r="A1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="18">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="M2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="N2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+      <c r="O2" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" s="2">
         <v>2</v>
@@ -694,25 +697,27 @@
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="P4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2">
         <v>5</v>
@@ -723,13 +728,13 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2">
         <v>6</v>
@@ -740,13 +745,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>7</v>
@@ -755,18 +760,18 @@
         <v>2</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -775,6 +780,7 @@
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added new functionality: update Products when importing if their SKU alredy exist in the database.
</commit_message>
<xml_diff>
--- a/uploads/data/import_products.xlsx
+++ b/uploads/data/import_products.xlsx
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>1007e2</t>
-  </si>
-  <si>
-    <t>1091e</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -84,49 +78,25 @@
     <t>Earrings</t>
   </si>
   <si>
-    <t>Rings</t>
-  </si>
-  <si>
-    <t>Sets</t>
-  </si>
-  <si>
-    <t>Pendant Green-Blue</t>
-  </si>
-  <si>
-    <t>Wonderful Earrings</t>
-  </si>
-  <si>
-    <t>Catherine the Great ring</t>
-  </si>
-  <si>
-    <t>Catherine the Great set</t>
-  </si>
-  <si>
-    <t>1076-5</t>
-  </si>
-  <si>
-    <t>1076-6</t>
-  </si>
-  <si>
-    <t>1076-7</t>
-  </si>
-  <si>
-    <t>honey</t>
-  </si>
-  <si>
     <t>product_category_id</t>
   </si>
   <si>
     <t>color_id</t>
   </si>
   <si>
-    <t>cognac</t>
-  </si>
-  <si>
-    <t>31903</t>
-  </si>
-  <si>
-    <t>Washka Pashka</t>
+    <t>24008-5</t>
+  </si>
+  <si>
+    <t>24008-6</t>
+  </si>
+  <si>
+    <t>Pendant Green-Blues 2</t>
+  </si>
+  <si>
+    <t>Some long description</t>
+  </si>
+  <si>
+    <t>Pendant Green-Blues Lamb</t>
   </si>
 </sst>
 </file>
@@ -171,10 +141,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -221,8 +190,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -234,23 +209,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,17 +561,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -603,175 +584,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
-      <c r="A1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" ht="18">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="N2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="P2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
+    <row r="3" spans="1:17" ht="17">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="1" t="s">
-        <v>34</v>
+    <row r="4" spans="1:17" ht="17">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="M5" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2">
-        <v>6</v>
-      </c>
-      <c r="N6" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2">
-        <v>7</v>
-      </c>
-      <c r="O7" s="2">
-        <v>2</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>